<commit_message>
EU-27 Updated InputData elec/BPHC, elec/BTaDLP
</commit_message>
<xml_diff>
--- a/InputData/elec/BPHC/BAU Pumped Hydro Cap.xlsx
+++ b/InputData/elec/BPHC/BAU Pumped Hydro Cap.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekte\2020\2020-04_EPS_Europe\30_Forschung_(intern)\InputData_EU28\elec\BPHC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Documents\eps-eu\InputData\elec\BPHC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CDABC6-B9CE-4E1F-86F0-566BCF3856DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0DC615-0745-4331-A6E3-955099CEF57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26190" yWindow="4140" windowWidth="19770" windowHeight="12945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="JRC_POTEnCIA" sheetId="5" r:id="rId2"/>
     <sheet name="BPHC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>BPHC BAU Pumped Hydro Capacity</t>
   </si>
@@ -44,16 +49,10 @@
     <t>Pumped Storage Capacity (MW)</t>
   </si>
   <si>
-    <t>EU28: Net capacities installed (MW)</t>
-  </si>
-  <si>
     <t>Pump storage</t>
   </si>
   <si>
     <t>JRC POTEnCIA</t>
-  </si>
-  <si>
-    <t>"Net Capacities", row 20</t>
   </si>
   <si>
     <t xml:space="preserve">Mantzos, L., Wiesenthal, T., Neuwahl, F., Rózsai, M., The POTEnCIA Central scenario: </t>
@@ -70,14 +69,23 @@
   <si>
     <t>Annual Reports, Power Generation, Central_2018_EU28_pg_det_yearly</t>
   </si>
+  <si>
+    <t>Annual Reports, Power Generation, Central_2018_UK_pg_det_yearly</t>
+  </si>
+  <si>
+    <t>EU27: Net capacities installed (MW)</t>
+  </si>
+  <si>
+    <t>"Net Capacities", row 52</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0;\-#,##0;&quot;-&quot;"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -284,12 +292,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -306,7 +314,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="6" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -317,8 +325,9 @@
     <cellStyle name="Font: Calibri, 9pt regular" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Header: bottom row" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Komma 2" xfId="15" xr:uid="{BF98F91E-DAE5-4389-A00B-280BD8B94D86}"/>
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal 2 2" xfId="9" xr:uid="{6666B3FF-4739-412C-AEB0-414853552E02}"/>
     <cellStyle name="Normal 2 3" xfId="11" xr:uid="{AA1E4ADB-8444-4C1E-86EA-D78F7D3A71E3}"/>
@@ -326,7 +335,6 @@
     <cellStyle name="Parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Percent 2" xfId="13" xr:uid="{BEAA776C-E47D-489A-865F-5A1E76D792BB}"/>
     <cellStyle name="Percent 3" xfId="14" xr:uid="{5114D1AE-FE94-4552-AE02-EAE0CCA9149F}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Table title" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -343,7 +351,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -665,70 +673,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{A12BA4F5-C71F-4F44-B342-A884746FF5E3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -737,14 +756,14 @@
   <dimension ref="A1:AZ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:52" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="52" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B1" s="7">
         <v>2000</v>
@@ -900,162 +919,162 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="8">
-        <v>41534.120000000003</v>
+        <v>38746.120000000003</v>
       </c>
       <c r="C2" s="8">
-        <v>41706.520000000004</v>
+        <v>38918.520000000004</v>
       </c>
       <c r="D2" s="8">
-        <v>41768.520000000004</v>
+        <v>38980.520000000004</v>
       </c>
       <c r="E2" s="8">
-        <v>41828.020000000004</v>
+        <v>39040.020000000004</v>
       </c>
       <c r="F2" s="8">
-        <v>42884.42</v>
+        <v>40096.42</v>
       </c>
       <c r="G2" s="8">
-        <v>43639.98</v>
+        <v>40851.980000000003</v>
       </c>
       <c r="H2" s="8">
-        <v>44038.58</v>
+        <v>41294.58</v>
       </c>
       <c r="I2" s="8">
-        <v>44038.58</v>
+        <v>41294.58</v>
       </c>
       <c r="J2" s="8">
-        <v>44316.58</v>
+        <v>41572.58</v>
       </c>
       <c r="K2" s="8">
-        <v>44712.58</v>
+        <v>41968.58</v>
       </c>
       <c r="L2" s="8">
-        <v>45071.38</v>
+        <v>42327.38</v>
       </c>
       <c r="M2" s="8">
-        <v>45311.38</v>
+        <v>42567.38</v>
       </c>
       <c r="N2" s="8">
-        <v>45486.48</v>
+        <v>42742.48</v>
       </c>
       <c r="O2" s="8">
-        <v>45915.48</v>
+        <v>43171.48</v>
       </c>
       <c r="P2" s="8">
-        <v>46268.480000000003</v>
+        <v>43524.480000000003</v>
       </c>
       <c r="Q2" s="8">
-        <v>47335.48</v>
+        <v>44591.48</v>
       </c>
       <c r="R2" s="8">
-        <v>47960.08</v>
+        <v>45216.08</v>
       </c>
       <c r="S2" s="8">
-        <v>48210.080000000002</v>
+        <v>45466.080000000002</v>
       </c>
       <c r="T2" s="8">
-        <v>48602.080000000002</v>
+        <v>45858.080000000002</v>
       </c>
       <c r="U2" s="8">
-        <v>48602.080000000002</v>
+        <v>45858.080000000002</v>
       </c>
       <c r="V2" s="8">
-        <v>48602.080000000002</v>
+        <v>45858.080000000002</v>
       </c>
       <c r="W2" s="8">
-        <v>48602.080000000002</v>
+        <v>45858.080000000002</v>
       </c>
       <c r="X2" s="8">
-        <v>48459.08</v>
+        <v>45715.08</v>
       </c>
       <c r="Y2" s="8">
-        <v>48359.08</v>
+        <v>45615.08</v>
       </c>
       <c r="Z2" s="8">
-        <v>48359.08</v>
+        <v>45615.08</v>
       </c>
       <c r="AA2" s="8">
-        <v>48359.08</v>
+        <v>45615.08</v>
       </c>
       <c r="AB2" s="8">
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="AC2" s="8">
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="AD2" s="8">
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="AE2" s="8">
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="AF2" s="8">
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="AG2" s="8">
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="AH2" s="8">
-        <v>48209.98</v>
+        <v>45465.98</v>
       </c>
       <c r="AI2" s="8">
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="AJ2" s="8">
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="AK2" s="8">
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="AL2" s="8">
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="AM2" s="8">
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="AN2" s="8">
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="AO2" s="8">
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="AP2" s="8">
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="AQ2" s="8">
-        <v>47969.98</v>
+        <v>45225.98</v>
       </c>
       <c r="AR2" s="8">
-        <v>47894.98</v>
+        <v>45150.98</v>
       </c>
       <c r="AS2" s="8">
-        <v>47894.98</v>
+        <v>45150.98</v>
       </c>
       <c r="AT2" s="8">
-        <v>47894.98</v>
+        <v>45150.98</v>
       </c>
       <c r="AU2" s="8">
-        <v>47828.98</v>
+        <v>45084.98</v>
       </c>
       <c r="AV2" s="8">
-        <v>47828.98</v>
+        <v>45084.98</v>
       </c>
       <c r="AW2" s="8">
-        <v>47828.98</v>
+        <v>45084.98</v>
       </c>
       <c r="AX2" s="8">
-        <v>47629.38</v>
+        <v>44885.38</v>
       </c>
       <c r="AY2" s="8">
-        <v>47577.120000000003</v>
+        <v>44833.120000000003</v>
       </c>
       <c r="AZ2" s="8">
-        <v>47488.160000000003</v>
+        <v>44744.160000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1071,15 +1090,15 @@
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1189,149 +1208,149 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4">
         <f>JRC_POTEnCIA!R2</f>
-        <v>47960.08</v>
+        <v>45216.08</v>
       </c>
       <c r="C2" s="4">
         <f>JRC_POTEnCIA!S2</f>
-        <v>48210.080000000002</v>
+        <v>45466.080000000002</v>
       </c>
       <c r="D2" s="4">
         <f>JRC_POTEnCIA!T2</f>
-        <v>48602.080000000002</v>
+        <v>45858.080000000002</v>
       </c>
       <c r="E2" s="4">
         <f>JRC_POTEnCIA!U2</f>
-        <v>48602.080000000002</v>
+        <v>45858.080000000002</v>
       </c>
       <c r="F2" s="4">
         <f>JRC_POTEnCIA!V2</f>
-        <v>48602.080000000002</v>
+        <v>45858.080000000002</v>
       </c>
       <c r="G2" s="4">
         <f>JRC_POTEnCIA!W2</f>
-        <v>48602.080000000002</v>
+        <v>45858.080000000002</v>
       </c>
       <c r="H2" s="4">
         <f>JRC_POTEnCIA!X2</f>
-        <v>48459.08</v>
+        <v>45715.08</v>
       </c>
       <c r="I2" s="4">
         <f>JRC_POTEnCIA!Y2</f>
-        <v>48359.08</v>
+        <v>45615.08</v>
       </c>
       <c r="J2" s="4">
         <f>JRC_POTEnCIA!Z2</f>
-        <v>48359.08</v>
+        <v>45615.08</v>
       </c>
       <c r="K2" s="4">
         <f>JRC_POTEnCIA!AA2</f>
-        <v>48359.08</v>
+        <v>45615.08</v>
       </c>
       <c r="L2" s="4">
         <f>JRC_POTEnCIA!AB2</f>
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="M2" s="4">
         <f>JRC_POTEnCIA!AC2</f>
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="N2" s="4">
         <f>JRC_POTEnCIA!AD2</f>
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="O2" s="4">
         <f>JRC_POTEnCIA!AE2</f>
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="P2" s="4">
         <f>JRC_POTEnCIA!AF2</f>
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="Q2" s="4">
         <f>JRC_POTEnCIA!AG2</f>
-        <v>48352.98</v>
+        <v>45608.98</v>
       </c>
       <c r="R2" s="4">
         <f>JRC_POTEnCIA!AH2</f>
-        <v>48209.98</v>
+        <v>45465.98</v>
       </c>
       <c r="S2" s="4">
         <f>JRC_POTEnCIA!AI2</f>
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="T2" s="4">
         <f>JRC_POTEnCIA!AJ2</f>
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="U2" s="4">
         <f>JRC_POTEnCIA!AK2</f>
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="V2" s="4">
         <f>JRC_POTEnCIA!AL2</f>
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="W2" s="4">
         <f>JRC_POTEnCIA!AM2</f>
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="X2" s="4">
         <f>JRC_POTEnCIA!AN2</f>
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="Y2" s="4">
         <f>JRC_POTEnCIA!AO2</f>
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="Z2" s="4">
         <f>JRC_POTEnCIA!AP2</f>
-        <v>48044.98</v>
+        <v>45300.98</v>
       </c>
       <c r="AA2" s="4">
         <f>JRC_POTEnCIA!AQ2</f>
-        <v>47969.98</v>
+        <v>45225.98</v>
       </c>
       <c r="AB2" s="4">
         <f>JRC_POTEnCIA!AR2</f>
-        <v>47894.98</v>
+        <v>45150.98</v>
       </c>
       <c r="AC2" s="4">
         <f>JRC_POTEnCIA!AS2</f>
-        <v>47894.98</v>
+        <v>45150.98</v>
       </c>
       <c r="AD2" s="4">
         <f>JRC_POTEnCIA!AT2</f>
-        <v>47894.98</v>
+        <v>45150.98</v>
       </c>
       <c r="AE2" s="4">
         <f>JRC_POTEnCIA!AU2</f>
-        <v>47828.98</v>
+        <v>45084.98</v>
       </c>
       <c r="AF2" s="4">
         <f>JRC_POTEnCIA!AV2</f>
-        <v>47828.98</v>
+        <v>45084.98</v>
       </c>
       <c r="AG2" s="4">
         <f>JRC_POTEnCIA!AW2</f>
-        <v>47828.98</v>
+        <v>45084.98</v>
       </c>
       <c r="AH2" s="4">
         <f>JRC_POTEnCIA!AX2</f>
-        <v>47629.38</v>
+        <v>44885.38</v>
       </c>
       <c r="AI2" s="4">
         <f>JRC_POTEnCIA!AY2</f>
-        <v>47577.120000000003</v>
+        <v>44833.120000000003</v>
       </c>
       <c r="AJ2" s="4">
         <f>JRC_POTEnCIA!AZ2</f>
-        <v>47488.160000000003</v>
+        <v>44744.160000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>